<commit_message>
Fix naming issues with the graphs
Add names to the graphs themselves and add missing axis names.
</commit_message>
<xml_diff>
--- a/MIT1/MSP/projekt/MSP_project.xlsx
+++ b/MIT1/MSP/projekt/MSP_project.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oraman\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oraman\Documents\MSP projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B22620-50A1-4FE0-B8B3-FA52FCACF71E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27718E7-1D82-44EB-A4E2-1800C932B751}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="4200" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="130">
   <si>
     <t>min</t>
   </si>
@@ -607,6 +607,12 @@
       </rPr>
       <t>NEZAMIETAM</t>
     </r>
+  </si>
+  <si>
+    <t>Početnosť</t>
+  </si>
+  <si>
+    <t>Teor. početnosť</t>
   </si>
 </sst>
 </file>
@@ -995,6 +1001,10 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1003,10 +1013,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -1055,7 +1061,7 @@
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t>Histogram - relatívnej četnosti</a:t>
+              <a:t>Histogram relatívnej početnosti</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1210,7 +1216,10 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="sk-SK"/>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Trieda</a:t>
+                </a:r>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1283,7 +1292,10 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="sk-SK"/>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Relatívna početnosť</a:t>
+                </a:r>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1316,25 +1328,6 @@
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0">
-            <a:defRPr b="0">
-              <a:solidFill>
-                <a:srgbClr val="1A1A1A"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="sk-SK"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
     <c:showDLblsOverMax val="1"/>
@@ -1375,7 +1368,7 @@
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t>Histogram - relatívnej kumulatívnej četnosti</a:t>
+              <a:t>Histogram relatívnej kumulatívnej početnosti</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1530,7 +1523,10 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="sk-SK"/>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Trieda</a:t>
+                </a:r>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1603,7 +1599,10 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="sk-SK"/>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Relatívna kumulatívna početnosť</a:t>
+                </a:r>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1636,25 +1635,6 @@
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0">
-            <a:defRPr b="0">
-              <a:solidFill>
-                <a:srgbClr val="1A1A1A"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="sk-SK"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
     <c:showDLblsOverMax val="1"/>
@@ -1695,7 +1675,7 @@
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t>Histogram - početnosti</a:t>
+              <a:t>Histogram početností</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1718,7 +1698,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>četnosť</c:v>
+                  <c:v>Početnosť</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1731,10 +1711,10 @@
           <c:invertIfNegative val="1"/>
           <c:cat>
             <c:numRef>
-              <c:f>Hárok1!$F$69:$F$74</c:f>
+              <c:f>Hárok1!$F$69:$F$75</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>-500.03590909090912</c:v>
                 </c:pt>
@@ -1752,16 +1732,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.830454545454546</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>501.02090909090907</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hárok1!$H$69:$H$74</c:f>
+              <c:f>Hárok1!$H$69:$H$75</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>9</c:v>
                 </c:pt>
@@ -1779,6 +1762,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1807,7 +1793,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Teor. četnosť</c:v>
+                  <c:v>Teor. početnosť</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1820,10 +1806,10 @@
           <c:invertIfNegative val="1"/>
           <c:cat>
             <c:numRef>
-              <c:f>Hárok1!$F$69:$F$74</c:f>
+              <c:f>Hárok1!$F$69:$F$75</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>-500.03590909090912</c:v>
                 </c:pt>
@@ -1841,16 +1827,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.830454545454546</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>501.02090909090907</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hárok1!$I$69:$I$74</c:f>
+              <c:f>Hárok1!$I$69:$I$75</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>7.9038315517296605</c:v>
                 </c:pt>
@@ -1868,6 +1857,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5.6658023406751079</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.9667653223789427</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1920,7 +1912,10 @@
                     <a:latin typeface="+mn-lt"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="sk-SK"/>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Stred triedy</a:t>
+                </a:r>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2080,10 +2075,7 @@
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2092,13 +2084,24 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Regresní</a:t>
+              <a:t>Regresn</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> přímka</a:t>
+              <a:rPr lang="sk-SK"/>
+              <a:t>á </a:t>
             </a:r>
-            <a:endParaRPr lang="en-GB"/>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>p</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="sk-SK"/>
+              <a:t>ria</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>mka</a:t>
+            </a:r>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2117,10 +2120,7 @@
           <a:pPr>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -2454,10 +2454,7 @@
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -2486,10 +2483,7 @@
               <a:pPr>
                 <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -2518,16 +2512,13 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="t" anchorCtr="1"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2571,10 +2562,7 @@
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -2603,10 +2591,7 @@
               <a:pPr>
                 <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -2641,10 +2626,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2697,7 +2679,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="sk-SK"/>
     </a:p>
@@ -2733,10 +2719,7 @@
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2745,7 +2728,39 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Pás spolehlivosti pro střední hodnotu</a:t>
+              <a:t>Pás spo</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="sk-SK"/>
+              <a:t>ľa</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>hlivosti pr</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="sk-SK"/>
+              <a:t>e</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t> st</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="sk-SK"/>
+              <a:t>r</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>edn</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="sk-SK"/>
+              <a:t>ú </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>hodnotu</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2765,10 +2780,7 @@
           <a:pPr>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -3340,10 +3352,7 @@
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -3372,10 +3381,7 @@
               <a:pPr>
                 <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -3410,10 +3416,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -3457,10 +3460,7 @@
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -3489,10 +3489,7 @@
               <a:pPr>
                 <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -3527,10 +3524,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -3583,7 +3577,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="sk-SK"/>
     </a:p>
@@ -3616,13 +3614,10 @@
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr>
+            <a:pPr algn="ctr" rtl="0">
               <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -3631,7 +3626,31 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Pás spolehlivosti pro individuální hodnotu</a:t>
+              <a:t>Pás spo</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="sk-SK"/>
+              <a:t>ľa</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>hlivosti pr</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="sk-SK"/>
+              <a:t>e</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t> individuáln</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="sk-SK"/>
+              <a:t>u</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t> hodnotu</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3648,13 +3667,10 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr>
+          <a:pPr algn="ctr" rtl="0">
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -4226,10 +4242,7 @@
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -4258,10 +4271,7 @@
               <a:pPr>
                 <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -4296,10 +4306,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -4343,10 +4350,7 @@
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -4375,10 +4379,7 @@
               <a:pPr>
                 <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -4413,10 +4414,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -4469,7 +4467,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="sk-SK"/>
     </a:p>
@@ -6154,10 +6156,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1724025</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>104776</xdr:rowOff>
+      <xdr:rowOff>76201</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5181600" cy="3028950"/>
     <xdr:graphicFrame macro="">
@@ -6570,8 +6572,8 @@
   </sheetPr>
   <dimension ref="A2:Y214"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F209" sqref="F209"/>
+    <sheetView topLeftCell="B64" workbookViewId="0">
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -7617,10 +7619,10 @@
         <v>15</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>16</v>
+        <v>128</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>31</v>
+        <v>129</v>
       </c>
       <c r="J68" s="2" t="s">
         <v>32</v>
@@ -9145,17 +9147,17 @@
   </sheetPr>
   <dimension ref="A1:R79"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E81" sqref="E81"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="H111" sqref="H111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A1" s="42">
+      <c r="A1" s="44">
         <v>3</v>
       </c>
-      <c r="B1" s="43"/>
+      <c r="B1" s="45"/>
     </row>
     <row r="2" spans="1:18" ht="15.75" customHeight="1">
       <c r="A2" s="4" t="s">
@@ -9199,8 +9201,8 @@
         <f>AVERAGE(B4:B23)</f>
         <v>82.920789156317596</v>
       </c>
-      <c r="K4" s="47"/>
-      <c r="M4" s="46"/>
+      <c r="K4" s="43"/>
+      <c r="M4" s="42"/>
     </row>
     <row r="5" spans="1:18" ht="14.25">
       <c r="A5" s="38">
@@ -9216,7 +9218,7 @@
         <f>SUMSQ(A4:A23)</f>
         <v>612014</v>
       </c>
-      <c r="K5" s="47"/>
+      <c r="K5" s="43"/>
     </row>
     <row r="6" spans="1:18" ht="14.25">
       <c r="A6" s="38">
@@ -9232,7 +9234,7 @@
         <f>SUMSQ(B4:B23)</f>
         <v>145333.4948086231</v>
       </c>
-      <c r="K6" s="47"/>
+      <c r="K6" s="43"/>
     </row>
     <row r="7" spans="1:18" ht="14.25">
       <c r="A7" s="38">
@@ -9248,7 +9250,7 @@
         <f>SUMPRODUCT(A4:A23,B4:B23)</f>
         <v>295053.9484981306</v>
       </c>
-      <c r="K7" s="47"/>
+      <c r="K7" s="43"/>
     </row>
     <row r="8" spans="1:18" ht="14.25">
       <c r="A8" s="38">
@@ -9257,7 +9259,7 @@
       <c r="B8" s="38">
         <v>108.81726243140818</v>
       </c>
-      <c r="K8" s="47"/>
+      <c r="K8" s="43"/>
     </row>
     <row r="9" spans="1:18" ht="14.25">
       <c r="A9" s="38">
@@ -9266,7 +9268,7 @@
       <c r="B9" s="38">
         <v>96.869579080583492</v>
       </c>
-      <c r="K9" s="47"/>
+      <c r="K9" s="43"/>
     </row>
     <row r="10" spans="1:18" ht="14.25">
       <c r="A10" s="38">
@@ -9275,7 +9277,7 @@
       <c r="B10" s="38">
         <v>58.291228804815773</v>
       </c>
-      <c r="K10" s="47"/>
+      <c r="K10" s="43"/>
     </row>
     <row r="11" spans="1:18" ht="14.25">
       <c r="A11" s="38">
@@ -9284,7 +9286,7 @@
       <c r="B11" s="38">
         <v>95.117538044840174</v>
       </c>
-      <c r="K11" s="47"/>
+      <c r="K11" s="43"/>
     </row>
     <row r="12" spans="1:18" ht="14.25">
       <c r="A12" s="38">
@@ -9293,7 +9295,7 @@
       <c r="B12" s="38">
         <v>97.749078257660415</v>
       </c>
-      <c r="K12" s="47"/>
+      <c r="K12" s="43"/>
     </row>
     <row r="13" spans="1:18" ht="14.25">
       <c r="A13" s="38">
@@ -9327,7 +9329,7 @@
       <c r="B14" s="38">
         <v>67.650352904768113</v>
       </c>
-      <c r="K14" s="47"/>
+      <c r="K14" s="43"/>
     </row>
     <row r="15" spans="1:18" ht="14.25">
       <c r="A15" s="38">
@@ -9343,7 +9345,7 @@
         <f>CORREL(A4:A23,B4:B23)</f>
         <v>0.93938112382659145</v>
       </c>
-      <c r="K15" s="47"/>
+      <c r="K15" s="43"/>
     </row>
     <row r="16" spans="1:18" ht="14.25">
       <c r="A16" s="38">
@@ -9352,7 +9354,7 @@
       <c r="B16" s="38">
         <v>85.406150991065601</v>
       </c>
-      <c r="K16" s="47"/>
+      <c r="K16" s="43"/>
     </row>
     <row r="17" spans="1:17" ht="14.25">
       <c r="A17" s="38">
@@ -9385,7 +9387,7 @@
       <c r="B18" s="38">
         <v>104.0342304661738</v>
       </c>
-      <c r="K18" s="47"/>
+      <c r="K18" s="43"/>
     </row>
     <row r="19" spans="1:17" ht="14.25">
       <c r="A19" s="38">
@@ -9400,7 +9402,7 @@
       <c r="E19" s="2">
         <v>0.05</v>
       </c>
-      <c r="K19" s="47"/>
+      <c r="K19" s="43"/>
     </row>
     <row r="20" spans="1:17" ht="14.25">
       <c r="A20" s="38">
@@ -9412,7 +9414,7 @@
       <c r="D20" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="K20" s="47"/>
+      <c r="K20" s="43"/>
     </row>
     <row r="21" spans="1:17" ht="14.25">
       <c r="A21" s="38">
@@ -9421,7 +9423,7 @@
       <c r="B21" s="38">
         <v>118.99800675675837</v>
       </c>
-      <c r="K21" s="47"/>
+      <c r="K21" s="43"/>
     </row>
     <row r="22" spans="1:17" ht="14.25">
       <c r="A22" s="38">
@@ -9437,7 +9439,7 @@
         <f>(F15*SQRT(F2-2))/SQRT(1-(F15*F15))</f>
         <v>11.623650930766503</v>
       </c>
-      <c r="K22" s="47"/>
+      <c r="K22" s="43"/>
     </row>
     <row r="23" spans="1:17" ht="14.25">
       <c r="A23" s="38">
@@ -9446,10 +9448,10 @@
       <c r="B23" s="38">
         <v>64.641799020289852</v>
       </c>
-      <c r="K23" s="47"/>
+      <c r="K23" s="43"/>
     </row>
     <row r="24" spans="1:17" ht="15">
-      <c r="B24" s="46"/>
+      <c r="B24" s="42"/>
       <c r="D24" s="31" t="s">
         <v>92</v>
       </c>
@@ -10086,14 +10088,14 @@
       </c>
     </row>
     <row r="67" spans="1:8" ht="12.75">
-      <c r="D67" s="44" t="s">
+      <c r="D67" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="E67" s="45"/>
-      <c r="F67" s="44" t="s">
+      <c r="E67" s="47"/>
+      <c r="F67" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="G67" s="45"/>
+      <c r="G67" s="47"/>
     </row>
     <row r="68" spans="1:8" ht="12.75">
       <c r="A68" s="21" t="s">

</xml_diff>

<commit_message>
Fix student weight input values for task 2
The values for the weights were incorrectly given by the tutor, as they
were decimal instead of being integers. After this fix, the calculations
as well as the regression graphs should be correct.
</commit_message>
<xml_diff>
--- a/MIT1/MSP/projekt/MSP_project.xlsx
+++ b/MIT1/MSP/projekt/MSP_project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oraman\Documents\MSP projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27718E7-1D82-44EB-A4E2-1800C932B751}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC32F018-65B5-40AE-9447-0F98D6CFB81E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2201,37 +2201,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>56.634502667378996</c:v>
+                  <c:v>56.43261237020937</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>62.088089075872489</c:v>
+                  <c:v>61.913398185518645</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>67.541675484365982</c:v>
+                  <c:v>67.394184000827892</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>72.995261892859475</c:v>
+                  <c:v>72.874969816137138</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>78.448848301352939</c:v>
+                  <c:v>78.355755631446414</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>83.902434709846432</c:v>
+                  <c:v>83.83654144675566</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>89.356021118339925</c:v>
+                  <c:v>89.317327262064907</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>94.809607526833418</c:v>
+                  <c:v>94.798113077374154</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>100.26319393532691</c:v>
+                  <c:v>100.27889889268343</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>105.7167803438204</c:v>
+                  <c:v>105.75968470799268</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>111.17036675231387</c:v>
+                  <c:v>111.24047052330192</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2342,64 +2342,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>67.092187854469032</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>52.275136156244642</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>78.472464405395215</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>57.281291138311616</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>108.81726243140818</c:v>
+                  <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>96.869579080583492</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>58.291228804815773</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>95.117538044840174</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>97.749078257660415</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>81.741693732823038</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>67.650352904768113</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>89.875038728747697</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>85.406150991065601</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>54.304659597564246</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>104.0342304661738</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>109.96838634967632</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>75.426975327530513</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>118.99800675675837</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>94.402723077225801</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>64.641799020289852</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2861,37 +2861,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>56.634502667378996</c:v>
+                  <c:v>56.43261237020937</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>62.088089075872489</c:v>
+                  <c:v>61.913398185518645</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>67.541675484365982</c:v>
+                  <c:v>67.394184000827892</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>72.995261892859475</c:v>
+                  <c:v>72.874969816137138</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>78.448848301352939</c:v>
+                  <c:v>78.355755631446414</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>83.902434709846432</c:v>
+                  <c:v>83.83654144675566</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>89.356021118339925</c:v>
+                  <c:v>89.317327262064907</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>94.809607526833418</c:v>
+                  <c:v>94.798113077374154</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>100.26319393532691</c:v>
+                  <c:v>100.27889889268343</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>105.7167803438204</c:v>
+                  <c:v>105.75968470799268</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>111.17036675231387</c:v>
+                  <c:v>111.24047052330192</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2980,37 +2980,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>50.817304689476828</c:v>
+                  <c:v>50.636888852685424</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>57.043790989775417</c:v>
+                  <c:v>56.887721363438601</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>63.183539855137752</c:v>
+                  <c:v>63.052136634582688</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>69.189345280774177</c:v>
+                  <c:v>69.083102924518556</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>74.99632625687623</c:v>
+                  <c:v>74.915978734741998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>80.541174858079415</c:v>
+                  <c:v>80.487689844077266</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>85.803630482633238</c:v>
+                  <c:v>85.778050443739758</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>90.824115991242778</c:v>
+                  <c:v>90.82733417153996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>95.670584824382985</c:v>
+                  <c:v>95.703243614626103</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>100.40234469874594</c:v>
+                  <c:v>100.46486755246012</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>105.05991291324402</c:v>
+                  <c:v>105.1525737124368</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3099,37 +3099,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>62.451700645281164</c:v>
+                  <c:v>62.228335887733316</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>67.132387161969561</c:v>
+                  <c:v>66.939075007598689</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>71.899811113594211</c:v>
+                  <c:v>71.736231367073103</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>76.801178504944772</c:v>
+                  <c:v>76.666836707755721</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>81.901370345829648</c:v>
+                  <c:v>81.795532528150829</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>87.263694561613448</c:v>
+                  <c:v>87.185393049434055</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>92.908411754046611</c:v>
+                  <c:v>92.856604080390056</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>98.795099062424057</c:v>
+                  <c:v>98.768891983208349</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>104.85580304627084</c:v>
+                  <c:v>104.85455417074076</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>111.03121598889487</c:v>
+                  <c:v>111.05450186352523</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>117.28082059138372</c:v>
+                  <c:v>117.32836733416704</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3240,64 +3240,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>67.092187854469032</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>52.275136156244642</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>78.472464405395215</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>57.281291138311616</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>108.81726243140818</c:v>
+                  <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>96.869579080583492</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>58.291228804815773</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>95.117538044840174</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>97.749078257660415</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>81.741693732823038</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>67.650352904768113</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>89.875038728747697</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>85.406150991065601</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>54.304659597564246</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>104.0342304661738</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>109.96838634967632</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>75.426975327530513</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>118.99800675675837</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>94.402723077225801</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>64.641799020289852</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3751,37 +3751,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>56.634502667378996</c:v>
+                  <c:v>56.43261237020937</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>62.088089075872489</c:v>
+                  <c:v>61.913398185518645</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>67.541675484365982</c:v>
+                  <c:v>67.394184000827892</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>72.995261892859475</c:v>
+                  <c:v>72.874969816137138</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>78.448848301352939</c:v>
+                  <c:v>78.355755631446414</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>83.902434709846432</c:v>
+                  <c:v>83.83654144675566</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>89.356021118339925</c:v>
+                  <c:v>89.317327262064907</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>94.809607526833418</c:v>
+                  <c:v>94.798113077374154</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>100.26319393532691</c:v>
+                  <c:v>100.27889889268343</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>105.7167803438204</c:v>
+                  <c:v>105.75968470799268</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>111.17036675231387</c:v>
+                  <c:v>111.24047052330192</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3870,37 +3870,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>40.535697293961583</c:v>
+                  <c:v>40.393236495227704</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>46.252158875266439</c:v>
+                  <c:v>46.135927067264106</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>51.91077377333815</c:v>
+                  <c:v>51.820984499823588</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>57.509244218996024</c:v>
+                  <c:v>57.446119506048674</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>63.045872919802079</c:v>
+                  <c:v>63.00964105913642</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>68.519658304783363</c:v>
+                  <c:v>68.510551285460195</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>73.930353503428705</c:v>
+                  <c:v>73.948604225843013</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79.278481202019464</c:v>
+                  <c:v>79.32432063704519</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>84.565302338587259</c:v>
+                  <c:v>84.638956802286245</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>89.79274290469391</c:v>
+                  <c:v>89.89443160323934</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>94.963288414239855</c:v>
+                  <c:v>95.093221378413332</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3989,37 +3989,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>72.733308040796402</c:v>
+                  <c:v>72.471988245191028</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>77.924019276478546</c:v>
+                  <c:v>77.690869303773184</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>83.172577195393814</c:v>
+                  <c:v>82.967383501832188</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>88.481279566722918</c:v>
+                  <c:v>88.303820126225602</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>93.851823682903799</c:v>
+                  <c:v>93.701870203756414</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>99.285211114909501</c:v>
+                  <c:v>99.162531608051125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>104.78168873325114</c:v>
+                  <c:v>104.6860502982868</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>110.34073385164737</c:v>
+                  <c:v>110.27190551770312</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>115.96108553206656</c:v>
+                  <c:v>115.91884098308061</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>121.6408177829469</c:v>
+                  <c:v>121.62493781274601</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>127.37744509038788</c:v>
+                  <c:v>127.38771966819051</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4130,64 +4130,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>67.092187854469032</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>52.275136156244642</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>78.472464405395215</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>57.281291138311616</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>108.81726243140818</c:v>
+                  <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>96.869579080583492</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>58.291228804815773</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>95.117538044840174</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>97.749078257660415</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>81.741693732823038</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>67.650352904768113</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>89.875038728747697</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>85.406150991065601</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>54.304659597564246</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>104.0342304661738</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>109.96838634967632</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>75.426975327530513</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>118.99800675675837</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>94.402723077225801</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>64.641799020289852</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9147,8 +9147,8 @@
   </sheetPr>
   <dimension ref="A1:R79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="H111" sqref="H111"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="J73" sqref="J73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -9192,14 +9192,14 @@
         <v>166</v>
       </c>
       <c r="B4" s="38">
-        <v>67.092187854469032</v>
+        <v>67</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>85</v>
       </c>
       <c r="F4" s="3">
         <f>AVERAGE(B4:B23)</f>
-        <v>82.920789156317596</v>
+        <v>82.85</v>
       </c>
       <c r="K4" s="43"/>
       <c r="M4" s="42"/>
@@ -9209,7 +9209,7 @@
         <v>152</v>
       </c>
       <c r="B5" s="38">
-        <v>52.275136156244642</v>
+        <v>52</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>86</v>
@@ -9225,14 +9225,14 @@
         <v>154</v>
       </c>
       <c r="B6" s="38">
-        <v>78.472464405395215</v>
+        <v>78</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>87</v>
       </c>
       <c r="F6" s="3">
         <f>SUMSQ(B4:B23)</f>
-        <v>145333.4948086231</v>
+        <v>145161</v>
       </c>
       <c r="K6" s="43"/>
     </row>
@@ -9241,14 +9241,14 @@
         <v>155</v>
       </c>
       <c r="B7" s="38">
-        <v>57.281291138311616</v>
+        <v>57</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>88</v>
       </c>
       <c r="F7" s="3">
         <f>SUMPRODUCT(A4:A23,B4:B23)</f>
-        <v>295053.9484981306</v>
+        <v>294839</v>
       </c>
       <c r="K7" s="43"/>
     </row>
@@ -9257,7 +9257,7 @@
         <v>190</v>
       </c>
       <c r="B8" s="38">
-        <v>108.81726243140818</v>
+        <v>109</v>
       </c>
       <c r="K8" s="43"/>
     </row>
@@ -9266,7 +9266,7 @@
         <v>182</v>
       </c>
       <c r="B9" s="38">
-        <v>96.869579080583492</v>
+        <v>97</v>
       </c>
       <c r="K9" s="43"/>
     </row>
@@ -9275,7 +9275,7 @@
         <v>153</v>
       </c>
       <c r="B10" s="38">
-        <v>58.291228804815773</v>
+        <v>58</v>
       </c>
       <c r="K10" s="43"/>
     </row>
@@ -9284,7 +9284,7 @@
         <v>193</v>
       </c>
       <c r="B11" s="38">
-        <v>95.117538044840174</v>
+        <v>95</v>
       </c>
       <c r="K11" s="43"/>
     </row>
@@ -9293,7 +9293,7 @@
         <v>191</v>
       </c>
       <c r="B12" s="38">
-        <v>97.749078257660415</v>
+        <v>98</v>
       </c>
       <c r="K12" s="43"/>
     </row>
@@ -9302,7 +9302,7 @@
         <v>166</v>
       </c>
       <c r="B13" s="38">
-        <v>81.741693732823038</v>
+        <v>82</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>10</v>
@@ -9327,7 +9327,7 @@
         <v>164</v>
       </c>
       <c r="B14" s="38">
-        <v>67.650352904768113</v>
+        <v>68</v>
       </c>
       <c r="K14" s="43"/>
     </row>
@@ -9336,14 +9336,14 @@
         <v>186</v>
       </c>
       <c r="B15" s="38">
-        <v>89.875038728747697</v>
+        <v>90</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>89</v>
       </c>
       <c r="F15" s="3">
         <f>CORREL(A4:A23,B4:B23)</f>
-        <v>0.93938112382659145</v>
+        <v>0.94033216833700461</v>
       </c>
       <c r="K15" s="43"/>
     </row>
@@ -9352,7 +9352,7 @@
         <v>175</v>
       </c>
       <c r="B16" s="38">
-        <v>85.406150991065601</v>
+        <v>85</v>
       </c>
       <c r="K16" s="43"/>
     </row>
@@ -9361,7 +9361,7 @@
         <v>154</v>
       </c>
       <c r="B17" s="38">
-        <v>54.304659597564246</v>
+        <v>54</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>19</v>
@@ -9385,7 +9385,7 @@
         <v>200</v>
       </c>
       <c r="B18" s="38">
-        <v>104.0342304661738</v>
+        <v>104</v>
       </c>
       <c r="K18" s="43"/>
     </row>
@@ -9394,7 +9394,7 @@
         <v>199</v>
       </c>
       <c r="B19" s="38">
-        <v>109.96838634967632</v>
+        <v>110</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>63</v>
@@ -9409,7 +9409,7 @@
         <v>164</v>
       </c>
       <c r="B20" s="38">
-        <v>75.426975327530513</v>
+        <v>75</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>90</v>
@@ -9421,7 +9421,7 @@
         <v>200</v>
       </c>
       <c r="B21" s="38">
-        <v>118.99800675675837</v>
+        <v>119</v>
       </c>
       <c r="K21" s="43"/>
     </row>
@@ -9430,14 +9430,14 @@
         <v>180</v>
       </c>
       <c r="B22" s="38">
-        <v>94.402723077225801</v>
+        <v>94</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>91</v>
       </c>
       <c r="E22" s="3">
         <f>(F15*SQRT(F2-2))/SQRT(1-(F15*F15))</f>
-        <v>11.623650930766503</v>
+        <v>11.724906175797353</v>
       </c>
       <c r="K22" s="43"/>
     </row>
@@ -9446,7 +9446,7 @@
         <v>158</v>
       </c>
       <c r="B23" s="38">
-        <v>64.641799020289852</v>
+        <v>65</v>
       </c>
       <c r="K23" s="43"/>
     </row>
@@ -9518,7 +9518,7 @@
         <v>166</v>
       </c>
       <c r="C43" s="7">
-        <v>67.092187854469032</v>
+        <v>67</v>
       </c>
       <c r="D43" s="3">
         <f t="shared" ref="D43:E43" si="0">B43*B43</f>
@@ -9526,11 +9526,11 @@
       </c>
       <c r="E43" s="3">
         <f t="shared" si="0"/>
-        <v>4501.361671099362</v>
+        <v>4489</v>
       </c>
       <c r="F43" s="3">
         <f t="shared" ref="F43:F62" si="1">B43*C43</f>
-        <v>11137.303183841859</v>
+        <v>11122</v>
       </c>
       <c r="H43" s="26" t="s">
         <v>100</v>
@@ -9541,7 +9541,7 @@
         <v>152</v>
       </c>
       <c r="C44" s="7">
-        <v>52.275136156244642</v>
+        <v>52</v>
       </c>
       <c r="D44" s="3">
         <f t="shared" ref="D44:E44" si="2">B44*B44</f>
@@ -9549,11 +9549,11 @@
       </c>
       <c r="E44" s="3">
         <f t="shared" si="2"/>
-        <v>2732.689860153916</v>
+        <v>2704</v>
       </c>
       <c r="F44" s="3">
         <f t="shared" si="1"/>
-        <v>7945.8206957491857</v>
+        <v>7904</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>101</v>
@@ -9568,7 +9568,7 @@
         <v>154</v>
       </c>
       <c r="C45" s="7">
-        <v>78.472464405395215</v>
+        <v>78</v>
       </c>
       <c r="D45" s="3">
         <f t="shared" ref="D45:E45" si="3">B45*B45</f>
@@ -9576,18 +9576,18 @@
       </c>
       <c r="E45" s="3">
         <f t="shared" si="3"/>
-        <v>6157.9276698560188</v>
+        <v>6084</v>
       </c>
       <c r="F45" s="3">
         <f t="shared" si="1"/>
-        <v>12084.759518430863</v>
+        <v>12012</v>
       </c>
       <c r="H45" s="9" t="s">
         <v>102</v>
       </c>
       <c r="I45" s="3">
         <f>(1/I44) * ((F2 * F63) - (B63 * C63))</f>
-        <v>1.0907172816986976</v>
+        <v>1.096157163061851</v>
       </c>
     </row>
     <row r="46" spans="1:17" ht="12.75">
@@ -9595,7 +9595,7 @@
         <v>155</v>
       </c>
       <c r="C46" s="7">
-        <v>57.281291138311616</v>
+        <v>57</v>
       </c>
       <c r="D46" s="3">
         <f t="shared" ref="D46:E46" si="4">B46*B46</f>
@@ -9603,18 +9603,18 @@
       </c>
       <c r="E46" s="3">
         <f t="shared" si="4"/>
-        <v>3281.1463144720169</v>
+        <v>3249</v>
       </c>
       <c r="F46" s="3">
         <f t="shared" si="1"/>
-        <v>8878.6001264383012</v>
+        <v>8835</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>103</v>
       </c>
       <c r="I46" s="3">
         <f>C64 - I45*B64</f>
-        <v>-106.97308958742565</v>
+        <v>-107.99096208906826</v>
       </c>
     </row>
     <row r="47" spans="1:17" ht="12.75">
@@ -9622,7 +9622,7 @@
         <v>190</v>
       </c>
       <c r="C47" s="7">
-        <v>108.81726243140818</v>
+        <v>109</v>
       </c>
       <c r="D47" s="3">
         <f t="shared" ref="D47:E47" si="5">B47*B47</f>
@@ -9630,11 +9630,11 @@
       </c>
       <c r="E47" s="3">
         <f t="shared" si="5"/>
-        <v>11841.196603065959</v>
+        <v>11881</v>
       </c>
       <c r="F47" s="3">
         <f t="shared" si="1"/>
-        <v>20675.279861967556</v>
+        <v>20710</v>
       </c>
       <c r="H47" s="2" t="s">
         <v>104</v>
@@ -9651,7 +9651,7 @@
         <v>182</v>
       </c>
       <c r="C48" s="7">
-        <v>96.869579080583492</v>
+        <v>97</v>
       </c>
       <c r="D48" s="3">
         <f t="shared" ref="D48:E48" si="6">B48*B48</f>
@@ -9659,18 +9659,18 @@
       </c>
       <c r="E48" s="3">
         <f t="shared" si="6"/>
-        <v>9383.7153512494187</v>
+        <v>9409</v>
       </c>
       <c r="F48" s="3">
         <f t="shared" si="1"/>
-        <v>17630.263392666195</v>
+        <v>17654</v>
       </c>
       <c r="H48" s="2" t="s">
         <v>107</v>
       </c>
       <c r="I48" s="3">
         <f>E63 - (I46 * C63) - (I45 * F63)</f>
-        <v>918.91428985050879</v>
+        <v>912.14238159306115</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="12.75">
@@ -9678,7 +9678,7 @@
         <v>153</v>
       </c>
       <c r="C49" s="7">
-        <v>58.291228804815773</v>
+        <v>58</v>
       </c>
       <c r="D49" s="3">
         <f t="shared" ref="D49:E49" si="7">B49*B49</f>
@@ -9686,18 +9686,18 @@
       </c>
       <c r="E49" s="3">
         <f t="shared" si="7"/>
-        <v>3397.867355575384</v>
+        <v>3364</v>
       </c>
       <c r="F49" s="3">
         <f t="shared" si="1"/>
-        <v>8918.5580071368131</v>
+        <v>8874</v>
       </c>
       <c r="H49" s="2" t="s">
         <v>108</v>
       </c>
       <c r="I49" s="3">
         <f>I48 / (F2 - 2)</f>
-        <v>51.050793880583825</v>
+        <v>50.674576755170065</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="12.75">
@@ -9705,7 +9705,7 @@
         <v>193</v>
       </c>
       <c r="C50" s="7">
-        <v>95.117538044840174</v>
+        <v>95</v>
       </c>
       <c r="D50" s="3">
         <f t="shared" ref="D50:E50" si="8">B50*B50</f>
@@ -9713,11 +9713,11 @@
       </c>
       <c r="E50" s="3">
         <f t="shared" si="8"/>
-        <v>9047.3460437116173</v>
+        <v>9025</v>
       </c>
       <c r="F50" s="3">
         <f t="shared" si="1"/>
-        <v>18357.684842654155</v>
+        <v>18335</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="12.75">
@@ -9725,7 +9725,7 @@
         <v>191</v>
       </c>
       <c r="C51" s="7">
-        <v>97.749078257660415</v>
+        <v>98</v>
       </c>
       <c r="D51" s="3">
         <f t="shared" ref="D51:E51" si="9">B51*B51</f>
@@ -9733,11 +9733,11 @@
       </c>
       <c r="E51" s="3">
         <f t="shared" si="9"/>
-        <v>9554.8823002222198</v>
+        <v>9604</v>
       </c>
       <c r="F51" s="3">
         <f t="shared" si="1"/>
-        <v>18670.073947213139</v>
+        <v>18718</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="12.75">
@@ -9745,7 +9745,7 @@
         <v>166</v>
       </c>
       <c r="C52" s="7">
-        <v>81.741693732823038</v>
+        <v>82</v>
       </c>
       <c r="D52" s="3">
         <f t="shared" ref="D52:E52" si="10">B52*B52</f>
@@ -9753,11 +9753,11 @@
       </c>
       <c r="E52" s="3">
         <f t="shared" si="10"/>
-        <v>6681.7044943106412</v>
+        <v>6724</v>
       </c>
       <c r="F52" s="3">
         <f t="shared" si="1"/>
-        <v>13569.121159648625</v>
+        <v>13612</v>
       </c>
       <c r="H52" s="26" t="s">
         <v>109</v>
@@ -9768,7 +9768,7 @@
         <v>164</v>
       </c>
       <c r="C53" s="7">
-        <v>67.650352904768113</v>
+        <v>68</v>
       </c>
       <c r="D53" s="3">
         <f t="shared" ref="D53:E53" si="11">B53*B53</f>
@@ -9776,11 +9776,11 @@
       </c>
       <c r="E53" s="3">
         <f t="shared" si="11"/>
-        <v>4576.5702481396675</v>
+        <v>4624</v>
       </c>
       <c r="F53" s="3">
         <f t="shared" si="1"/>
-        <v>11094.657876381971</v>
+        <v>11152</v>
       </c>
       <c r="H53" s="2" t="s">
         <v>110</v>
@@ -9794,7 +9794,7 @@
         <v>186</v>
       </c>
       <c r="C54" s="7">
-        <v>89.875038728747697</v>
+        <v>90</v>
       </c>
       <c r="D54" s="3">
         <f t="shared" ref="D54:E54" si="12">B54*B54</f>
@@ -9802,11 +9802,11 @@
       </c>
       <c r="E54" s="3">
         <f t="shared" si="12"/>
-        <v>8077.5225864938984</v>
+        <v>8100</v>
       </c>
       <c r="F54" s="3">
         <f t="shared" si="1"/>
-        <v>16716.757203547073</v>
+        <v>16740</v>
       </c>
       <c r="H54" s="9" t="s">
         <v>111</v>
@@ -9820,7 +9820,7 @@
         <v>175</v>
       </c>
       <c r="C55" s="7">
-        <v>85.406150991065601</v>
+        <v>85</v>
       </c>
       <c r="D55" s="3">
         <f t="shared" ref="D55:E55" si="13">B55*B55</f>
@@ -9828,11 +9828,11 @@
       </c>
       <c r="E55" s="3">
         <f t="shared" si="13"/>
-        <v>7294.2106271086959</v>
+        <v>7225</v>
       </c>
       <c r="F55" s="3">
         <f t="shared" si="1"/>
-        <v>14946.07642343648</v>
+        <v>14875</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>112</v>
@@ -9847,7 +9847,7 @@
         <v>154</v>
       </c>
       <c r="C56" s="7">
-        <v>54.304659597564246</v>
+        <v>54</v>
       </c>
       <c r="D56" s="3">
         <f t="shared" ref="D56:E56" si="14">B56*B56</f>
@@ -9855,18 +9855,18 @@
       </c>
       <c r="E56" s="3">
         <f t="shared" si="14"/>
-        <v>2948.9960540073266</v>
+        <v>2916</v>
       </c>
       <c r="F56" s="3">
         <f t="shared" si="1"/>
-        <v>8362.9175780248934</v>
+        <v>8316</v>
       </c>
       <c r="H56" s="2" t="s">
         <v>62</v>
       </c>
       <c r="I56" s="3">
         <f>(I46-(-100))/(SQRT(I49)*SQRT(I55))</f>
-        <v>-0.42480530263053357</v>
+        <v>-0.48861853765211893</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="12.75">
@@ -9874,7 +9874,7 @@
         <v>200</v>
       </c>
       <c r="C57" s="7">
-        <v>104.0342304661738</v>
+        <v>104</v>
       </c>
       <c r="D57" s="3">
         <f t="shared" ref="D57:E57" si="15">B57*B57</f>
@@ -9882,11 +9882,11 @@
       </c>
       <c r="E57" s="3">
         <f t="shared" si="15"/>
-        <v>10823.121108688963</v>
+        <v>10816</v>
       </c>
       <c r="F57" s="3">
         <f t="shared" si="1"/>
-        <v>20806.846093234759</v>
+        <v>20800</v>
       </c>
       <c r="H57" s="2" t="s">
         <v>92</v>
@@ -9901,7 +9901,7 @@
         <v>199</v>
       </c>
       <c r="C58" s="7">
-        <v>109.96838634967632</v>
+        <v>110</v>
       </c>
       <c r="D58" s="3">
         <f t="shared" ref="D58:E58" si="16">B58*B58</f>
@@ -9909,11 +9909,11 @@
       </c>
       <c r="E58" s="3">
         <f t="shared" si="16"/>
-        <v>12093.045996351677</v>
+        <v>12100</v>
       </c>
       <c r="F58" s="3">
         <f t="shared" si="1"/>
-        <v>21883.708883585587</v>
+        <v>21890</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>93</v>
@@ -9928,7 +9928,7 @@
         <v>164</v>
       </c>
       <c r="C59" s="7">
-        <v>75.426975327530513</v>
+        <v>75</v>
       </c>
       <c r="D59" s="3">
         <f t="shared" ref="D59:E59" si="17">B59*B59</f>
@@ -9936,11 +9936,11 @@
       </c>
       <c r="E59" s="3">
         <f t="shared" si="17"/>
-        <v>5689.2286070598966</v>
+        <v>5625</v>
       </c>
       <c r="F59" s="3">
         <f t="shared" si="1"/>
-        <v>12370.023953715005</v>
+        <v>12300</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>113</v>
@@ -9951,7 +9951,7 @@
         <v>200</v>
       </c>
       <c r="C60" s="7">
-        <v>118.99800675675837</v>
+        <v>119</v>
       </c>
       <c r="D60" s="3">
         <f t="shared" ref="D60:E60" si="18">B60*B60</f>
@@ -9959,11 +9959,11 @@
       </c>
       <c r="E60" s="3">
         <f t="shared" si="18"/>
-        <v>14160.52561208151</v>
+        <v>14161</v>
       </c>
       <c r="F60" s="3">
         <f t="shared" si="1"/>
-        <v>23799.601351351674</v>
+        <v>23800</v>
       </c>
       <c r="H60" s="2" t="s">
         <v>64</v>
@@ -9978,7 +9978,7 @@
         <v>180</v>
       </c>
       <c r="C61" s="7">
-        <v>94.402723077225801</v>
+        <v>94</v>
       </c>
       <c r="D61" s="3">
         <f t="shared" ref="D61:E61" si="19">B61*B61</f>
@@ -9986,11 +9986,11 @@
       </c>
       <c r="E61" s="3">
         <f t="shared" si="19"/>
-        <v>8911.8741243953809</v>
+        <v>8836</v>
       </c>
       <c r="F61" s="3">
         <f t="shared" si="1"/>
-        <v>16992.490153900646</v>
+        <v>16920</v>
       </c>
       <c r="H61" s="2" t="s">
         <v>114</v>
@@ -10005,7 +10005,7 @@
         <v>158</v>
       </c>
       <c r="C62" s="7">
-        <v>64.641799020289852</v>
+        <v>65</v>
       </c>
       <c r="D62" s="3">
         <f t="shared" ref="D62:E62" si="20">B62*B62</f>
@@ -10013,18 +10013,18 @@
       </c>
       <c r="E62" s="3">
         <f t="shared" si="20"/>
-        <v>4178.5621805795463</v>
+        <v>4225</v>
       </c>
       <c r="F62" s="3">
         <f t="shared" si="1"/>
-        <v>10213.404245205797</v>
+        <v>10270</v>
       </c>
       <c r="H62" s="2" t="s">
         <v>115</v>
       </c>
       <c r="I62" s="3">
         <f>($I$45-1)/(SQRT($I$49)*SQRT($I$61))</f>
-        <v>0.96676382922204718</v>
+        <v>1.0285329084397048</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="12.75">
@@ -10037,7 +10037,7 @@
       </c>
       <c r="C63" s="35">
         <f t="shared" si="21"/>
-        <v>1658.4157831263519</v>
+        <v>1657</v>
       </c>
       <c r="D63" s="35">
         <f t="shared" si="21"/>
@@ -10045,11 +10045,11 @@
       </c>
       <c r="E63" s="35">
         <f t="shared" si="21"/>
-        <v>145333.4948086231</v>
+        <v>145161</v>
       </c>
       <c r="F63" s="36">
         <f t="shared" si="21"/>
-        <v>295053.9484981306</v>
+        <v>294839</v>
       </c>
       <c r="H63" s="2" t="s">
         <v>92</v>
@@ -10069,7 +10069,7 @@
       </c>
       <c r="C64" s="35">
         <f t="shared" si="22"/>
-        <v>82.920789156317596</v>
+        <v>82.85</v>
       </c>
       <c r="D64" s="35"/>
       <c r="E64" s="35"/>
@@ -10129,23 +10129,23 @@
       </c>
       <c r="C69" s="3">
         <f t="shared" ref="C69:C79" si="23">$I$45*B69+$I$46</f>
-        <v>56.634502667378996</v>
+        <v>56.43261237020937</v>
       </c>
       <c r="D69" s="3">
         <f t="shared" ref="D69:D79" si="24">C69-$I$57*SQRT($I$49)*SQRT(H69)</f>
-        <v>50.817304689476828</v>
+        <v>50.636888852685424</v>
       </c>
       <c r="E69" s="3">
         <f t="shared" ref="E69:E79" si="25">C69+$I$57*SQRT($I$49)*SQRT(H69)</f>
-        <v>62.451700645281164</v>
+        <v>62.228335887733316</v>
       </c>
       <c r="F69" s="3">
         <f t="shared" ref="F69:F79" si="26">C69-$I$57*SQRT($I$49)*SQRT(H69+1)</f>
-        <v>40.535697293961583</v>
+        <v>40.393236495227704</v>
       </c>
       <c r="G69" s="3">
         <f t="shared" ref="G69:G79" si="27">C69+$I$57*SQRT($I$49)*SQRT(H69+1)</f>
-        <v>72.733308040796402</v>
+        <v>72.471988245191028</v>
       </c>
       <c r="H69" s="2">
         <f t="shared" ref="H69:H79" si="28">1/$I$60+(($I$60*(B69-$B$64)^2)/$I$44)</f>
@@ -10158,23 +10158,23 @@
       </c>
       <c r="C70" s="3">
         <f t="shared" si="23"/>
-        <v>62.088089075872489</v>
+        <v>61.913398185518645</v>
       </c>
       <c r="D70" s="3">
         <f t="shared" si="24"/>
-        <v>57.043790989775417</v>
+        <v>56.887721363438601</v>
       </c>
       <c r="E70" s="3">
         <f t="shared" si="25"/>
-        <v>67.132387161969561</v>
+        <v>66.939075007598689</v>
       </c>
       <c r="F70" s="3">
         <f t="shared" si="26"/>
-        <v>46.252158875266439</v>
+        <v>46.135927067264106</v>
       </c>
       <c r="G70" s="3">
         <f t="shared" si="27"/>
-        <v>77.924019276478546</v>
+        <v>77.690869303773184</v>
       </c>
       <c r="H70" s="2">
         <f t="shared" si="28"/>
@@ -10187,23 +10187,23 @@
       </c>
       <c r="C71" s="3">
         <f t="shared" si="23"/>
-        <v>67.541675484365982</v>
+        <v>67.394184000827892</v>
       </c>
       <c r="D71" s="3">
         <f t="shared" si="24"/>
-        <v>63.183539855137752</v>
+        <v>63.052136634582688</v>
       </c>
       <c r="E71" s="3">
         <f t="shared" si="25"/>
-        <v>71.899811113594211</v>
+        <v>71.736231367073103</v>
       </c>
       <c r="F71" s="3">
         <f t="shared" si="26"/>
-        <v>51.91077377333815</v>
+        <v>51.820984499823588</v>
       </c>
       <c r="G71" s="3">
         <f t="shared" si="27"/>
-        <v>83.172577195393814</v>
+        <v>82.967383501832188</v>
       </c>
       <c r="H71" s="2">
         <f t="shared" si="28"/>
@@ -10216,23 +10216,23 @@
       </c>
       <c r="C72" s="3">
         <f t="shared" si="23"/>
-        <v>72.995261892859475</v>
+        <v>72.874969816137138</v>
       </c>
       <c r="D72" s="3">
         <f t="shared" si="24"/>
-        <v>69.189345280774177</v>
+        <v>69.083102924518556</v>
       </c>
       <c r="E72" s="3">
         <f t="shared" si="25"/>
-        <v>76.801178504944772</v>
+        <v>76.666836707755721</v>
       </c>
       <c r="F72" s="3">
         <f t="shared" si="26"/>
-        <v>57.509244218996024</v>
+        <v>57.446119506048674</v>
       </c>
       <c r="G72" s="3">
         <f t="shared" si="27"/>
-        <v>88.481279566722918</v>
+        <v>88.303820126225602</v>
       </c>
       <c r="H72" s="2">
         <f t="shared" si="28"/>
@@ -10245,23 +10245,23 @@
       </c>
       <c r="C73" s="3">
         <f t="shared" si="23"/>
-        <v>78.448848301352939</v>
+        <v>78.355755631446414</v>
       </c>
       <c r="D73" s="3">
         <f t="shared" si="24"/>
-        <v>74.99632625687623</v>
+        <v>74.915978734741998</v>
       </c>
       <c r="E73" s="3">
         <f t="shared" si="25"/>
-        <v>81.901370345829648</v>
+        <v>81.795532528150829</v>
       </c>
       <c r="F73" s="3">
         <f t="shared" si="26"/>
-        <v>63.045872919802079</v>
+        <v>63.00964105913642</v>
       </c>
       <c r="G73" s="3">
         <f t="shared" si="27"/>
-        <v>93.851823682903799</v>
+        <v>93.701870203756414</v>
       </c>
       <c r="H73" s="2">
         <f t="shared" si="28"/>
@@ -10274,23 +10274,23 @@
       </c>
       <c r="C74" s="3">
         <f t="shared" si="23"/>
-        <v>83.902434709846432</v>
+        <v>83.83654144675566</v>
       </c>
       <c r="D74" s="3">
         <f t="shared" si="24"/>
-        <v>80.541174858079415</v>
+        <v>80.487689844077266</v>
       </c>
       <c r="E74" s="3">
         <f t="shared" si="25"/>
-        <v>87.263694561613448</v>
+        <v>87.185393049434055</v>
       </c>
       <c r="F74" s="3">
         <f t="shared" si="26"/>
-        <v>68.519658304783363</v>
+        <v>68.510551285460195</v>
       </c>
       <c r="G74" s="3">
         <f t="shared" si="27"/>
-        <v>99.285211114909501</v>
+        <v>99.162531608051125</v>
       </c>
       <c r="H74" s="2">
         <f t="shared" si="28"/>
@@ -10303,23 +10303,23 @@
       </c>
       <c r="C75" s="3">
         <f t="shared" si="23"/>
-        <v>89.356021118339925</v>
+        <v>89.317327262064907</v>
       </c>
       <c r="D75" s="3">
         <f t="shared" si="24"/>
-        <v>85.803630482633238</v>
+        <v>85.778050443739758</v>
       </c>
       <c r="E75" s="3">
         <f t="shared" si="25"/>
-        <v>92.908411754046611</v>
+        <v>92.856604080390056</v>
       </c>
       <c r="F75" s="3">
         <f t="shared" si="26"/>
-        <v>73.930353503428705</v>
+        <v>73.948604225843013</v>
       </c>
       <c r="G75" s="3">
         <f t="shared" si="27"/>
-        <v>104.78168873325114</v>
+        <v>104.6860502982868</v>
       </c>
       <c r="H75" s="2">
         <f t="shared" si="28"/>
@@ -10332,23 +10332,23 @@
       </c>
       <c r="C76" s="3">
         <f t="shared" si="23"/>
-        <v>94.809607526833418</v>
+        <v>94.798113077374154</v>
       </c>
       <c r="D76" s="3">
         <f t="shared" si="24"/>
-        <v>90.824115991242778</v>
+        <v>90.82733417153996</v>
       </c>
       <c r="E76" s="3">
         <f t="shared" si="25"/>
-        <v>98.795099062424057</v>
+        <v>98.768891983208349</v>
       </c>
       <c r="F76" s="3">
         <f t="shared" si="26"/>
-        <v>79.278481202019464</v>
+        <v>79.32432063704519</v>
       </c>
       <c r="G76" s="3">
         <f t="shared" si="27"/>
-        <v>110.34073385164737</v>
+        <v>110.27190551770312</v>
       </c>
       <c r="H76" s="2">
         <f t="shared" si="28"/>
@@ -10361,23 +10361,23 @@
       </c>
       <c r="C77" s="3">
         <f t="shared" si="23"/>
-        <v>100.26319393532691</v>
+        <v>100.27889889268343</v>
       </c>
       <c r="D77" s="3">
         <f t="shared" si="24"/>
-        <v>95.670584824382985</v>
+        <v>95.703243614626103</v>
       </c>
       <c r="E77" s="3">
         <f t="shared" si="25"/>
-        <v>104.85580304627084</v>
+        <v>104.85455417074076</v>
       </c>
       <c r="F77" s="3">
         <f t="shared" si="26"/>
-        <v>84.565302338587259</v>
+        <v>84.638956802286245</v>
       </c>
       <c r="G77" s="3">
         <f t="shared" si="27"/>
-        <v>115.96108553206656</v>
+        <v>115.91884098308061</v>
       </c>
       <c r="H77" s="2">
         <f t="shared" si="28"/>
@@ -10390,23 +10390,23 @@
       </c>
       <c r="C78" s="3">
         <f t="shared" si="23"/>
-        <v>105.7167803438204</v>
+        <v>105.75968470799268</v>
       </c>
       <c r="D78" s="3">
         <f t="shared" si="24"/>
-        <v>100.40234469874594</v>
+        <v>100.46486755246012</v>
       </c>
       <c r="E78" s="3">
         <f t="shared" si="25"/>
-        <v>111.03121598889487</v>
+        <v>111.05450186352523</v>
       </c>
       <c r="F78" s="3">
         <f t="shared" si="26"/>
-        <v>89.79274290469391</v>
+        <v>89.89443160323934</v>
       </c>
       <c r="G78" s="3">
         <f t="shared" si="27"/>
-        <v>121.6408177829469</v>
+        <v>121.62493781274601</v>
       </c>
       <c r="H78" s="2">
         <f t="shared" si="28"/>
@@ -10419,23 +10419,23 @@
       </c>
       <c r="C79" s="3">
         <f t="shared" si="23"/>
-        <v>111.17036675231387</v>
+        <v>111.24047052330192</v>
       </c>
       <c r="D79" s="3">
         <f t="shared" si="24"/>
-        <v>105.05991291324402</v>
+        <v>105.1525737124368</v>
       </c>
       <c r="E79" s="3">
         <f t="shared" si="25"/>
-        <v>117.28082059138372</v>
+        <v>117.32836733416704</v>
       </c>
       <c r="F79" s="3">
         <f t="shared" si="26"/>
-        <v>94.963288414239855</v>
+        <v>95.093221378413332</v>
       </c>
       <c r="G79" s="3">
         <f t="shared" si="27"/>
-        <v>127.37744509038788</v>
+        <v>127.38771966819051</v>
       </c>
       <c r="H79" s="2">
         <f t="shared" si="28"/>

</xml_diff>

<commit_message>
Fix incorrect calculation in subtask g) of task 1
The variances and standard deviations of the two datasets are now
calculated as samples (bodovy odhad) instead of as based on the entire
population (populacny odhad). This fixes the testing criterium as well,
as it uses the estimated sample variance result. These values are fixed
in the documentation as well.
</commit_message>
<xml_diff>
--- a/MIT1/MSP/projekt/MSP_project.xlsx
+++ b/MIT1/MSP/projekt/MSP_project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oraman\Documents\MSP projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC32F018-65B5-40AE-9447-0F98D6CFB81E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6497350B-59C8-49A4-9ADE-79BD2781F743}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -6572,8 +6572,8 @@
   </sheetPr>
   <dimension ref="A2:Y214"/>
   <sheetViews>
-    <sheetView topLeftCell="B64" workbookViewId="0">
-      <selection activeCell="F86" sqref="F86"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="C198" sqref="C198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -8912,7 +8912,7 @@
       </c>
       <c r="F192" s="22">
         <f>B197/C197</f>
-        <v>0.55145197159791892</v>
+        <v>0.56112656759086477</v>
       </c>
       <c r="G192" s="22"/>
       <c r="H192" s="22"/>
@@ -8987,12 +8987,12 @@
         <v>67</v>
       </c>
       <c r="B197" s="3">
-        <f>VARP(B163:B182)</f>
-        <v>0.6287299999999999</v>
+        <f>_xlfn.VAR.S(B163:B182)</f>
+        <v>0.66182105263157875</v>
       </c>
       <c r="C197" s="2">
-        <f>VARP(C163:C192)</f>
-        <v>1.1401355555555559</v>
+        <f>_xlfn.VAR.S(C163:C192)</f>
+        <v>1.179450574712644</v>
       </c>
       <c r="E197" s="21" t="s">
         <v>68</v>
@@ -9006,12 +9006,12 @@
         <v>69</v>
       </c>
       <c r="B198" s="2">
-        <f>_xlfn.STDEV.P(B163:B182)</f>
-        <v>0.7929249649241723</v>
+        <f>_xlfn.STDEV.S(B163:B182)</f>
+        <v>0.81352384884008089</v>
       </c>
       <c r="C198" s="2">
-        <f>_xlfn.STDEV.P(C163:C192)</f>
-        <v>1.0677713030211835</v>
+        <f>_xlfn.STDEV.S(C163:C192)</f>
+        <v>1.0860251261884524</v>
       </c>
     </row>
     <row r="200" spans="1:8" ht="12.75">
@@ -9104,7 +9104,7 @@
       </c>
       <c r="F208" s="22">
         <f>((B196-C196-F207) / SQRT(((B195-1)*B197) +((C195-1)*C197))) * (SQRT(((B195*C195)*(B195+C195-2)) / (B195+C195)))</f>
-        <v>1.9436767711640788</v>
+        <v>1.9065740249458809</v>
       </c>
       <c r="G208" s="27"/>
       <c r="H208" s="22"/>
@@ -9147,8 +9147,8 @@
   </sheetPr>
   <dimension ref="A1:R79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="J73" sqref="J73"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>